<commit_message>
Added three solar system cards.
</commit_message>
<xml_diff>
--- a/Software Engineering/templates/Software Design Database.xlsx
+++ b/Software Engineering/templates/Software Design Database.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tyler\git\conquer\Software Engineering\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAEE06F5-FE96-4695-BEF1-8D50FE9514EC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="161">
   <si>
     <t>idx</t>
   </si>
@@ -481,12 +475,39 @@
   </si>
   <si>
     <t>Glows from space. Hopefully it is gold</t>
+  </si>
+  <si>
+    <t>Appert System</t>
+  </si>
+  <si>
+    <t>Appert System.png</t>
+  </si>
+  <si>
+    <t>Cartof System</t>
+  </si>
+  <si>
+    <t>Cartof System.png</t>
+  </si>
+  <si>
+    <t>VanWeiss System</t>
+  </si>
+  <si>
+    <t>VanWeiss System.png</t>
+  </si>
+  <si>
+    <t>Do not mess with us</t>
+  </si>
+  <si>
+    <t>We only like peaceful people here</t>
+  </si>
+  <si>
+    <t>Almost time travels through space</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -843,36 +864,36 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J47"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25:H47"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="J51" sqref="J51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7" style="2" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="2"/>
+    <col min="2" max="2" width="8.85546875" style="2"/>
     <col min="3" max="3" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="25.109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="29.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.33203125" style="4" customWidth="1"/>
-    <col min="9" max="9" width="30.33203125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="17.5546875" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="2"/>
+    <col min="4" max="4" width="19.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="29.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.28515625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="30.28515625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="17.5703125" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -904,7 +925,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -936,7 +957,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -968,7 +989,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1000,7 +1021,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1032,7 +1053,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1064,7 +1085,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1096,7 +1117,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1128,7 +1149,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1160,7 +1181,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1192,7 +1213,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1224,7 +1245,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1256,7 +1277,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1288,7 +1309,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1320,7 +1341,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1352,7 +1373,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1384,7 +1405,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1416,7 +1437,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1448,7 +1469,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1480,7 +1501,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1512,7 +1533,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -1544,7 +1565,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -1576,7 +1597,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -1608,7 +1629,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -1640,7 +1661,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -1672,7 +1693,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -1704,7 +1725,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -1736,7 +1757,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -1768,7 +1789,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -1800,7 +1821,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -1832,7 +1853,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -1864,7 +1885,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -1896,7 +1917,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -1928,7 +1949,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -1960,7 +1981,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -1992,7 +2013,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -2024,7 +2045,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -2056,7 +2077,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -2088,7 +2109,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -2120,7 +2141,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -2152,7 +2173,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -2184,7 +2205,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -2216,7 +2237,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -2248,7 +2269,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -2280,7 +2301,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -2312,7 +2333,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -2344,7 +2365,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -2374,6 +2395,102 @@
       </c>
       <c r="J47" s="2">
         <v>300</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A48" s="2">
+        <v>47</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="F48" s="2">
+        <v>5</v>
+      </c>
+      <c r="G48" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="H48" s="4">
+        <v>0.03</v>
+      </c>
+      <c r="I48" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="J48" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A49" s="2">
+        <v>48</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="F49" s="2">
+        <v>5</v>
+      </c>
+      <c r="G49" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="H49" s="4">
+        <v>0.03</v>
+      </c>
+      <c r="I49" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="J49" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A50" s="2">
+        <v>49</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="F50" s="2">
+        <v>5</v>
+      </c>
+      <c r="G50" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="H50" s="4">
+        <v>0.03</v>
+      </c>
+      <c r="I50" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="J50" s="2">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>